<commit_message>
added csv and excel
</commit_message>
<xml_diff>
--- a/data/MASTER Krypton Literature Review.xlsx
+++ b/data/MASTER Krypton Literature Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23076523_student_uwa_edu_au/Documents/MPE Engineering Research Project GENG5511.2/TOTAL LIT DATA REVIEWS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23059859_student_uwa_edu_au/Documents/UWA/05. Year 5/Semester 1/GENG5511 MPE Engineering Research Project/Project/Research_Project/GENG5511_Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{203C6214-688B-46A2-910E-DA614D10E36E}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EA16B5B-F567-4016-80B1-C299924FB7FE}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11295" firstSheet="7" activeTab="2" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell Volume " sheetId="1" r:id="rId1"/>
@@ -1394,14 +1394,23 @@
     <xf numFmtId="4" fontId="21" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1421,15 +1430,6 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1444,8 +1444,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1784,17 +1784,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F513A9-1C82-3E45-A361-2C7180831D5E}">
   <dimension ref="A1:AE136"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="6.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.08203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
@@ -1804,33 +1804,33 @@
     <col min="11" max="11" width="12.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.08203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.75" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.25" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.58203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.5" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="4.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:27">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="26" t="s">
         <v>1</v>
       </c>
@@ -1853,19 +1853,19 @@
       <c r="Z1" s="21"/>
       <c r="AA1" s="21"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75">
+    <row r="2" spans="1:27">
       <c r="A2" s="5"/>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="2">
         <f>6.02214076*10^23</f>
         <v>6.0221407599999999E+23</v>
@@ -1889,8 +1889,8 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75">
-      <c r="A3" s="61" t="s">
+    <row r="3" spans="1:27">
+      <c r="A3" s="64" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="56" t="s">
@@ -1918,7 +1918,7 @@
       <c r="J3" s="56"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="61" t="s">
+      <c r="M3" s="64" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="56" t="s">
@@ -1952,8 +1952,8 @@
       </c>
       <c r="AA3" s="56"/>
     </row>
-    <row r="4" spans="1:27" ht="18">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:27" ht="16.5">
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -1963,10 +1963,10 @@
       <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="57"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="7" t="s">
         <v>17</v>
       </c>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="61"/>
+      <c r="M4" s="64"/>
       <c r="N4" s="56"/>
       <c r="O4" s="56"/>
       <c r="P4" s="56"/>
@@ -1989,12 +1989,12 @@
         <v>16</v>
       </c>
       <c r="T4" s="7"/>
-      <c r="U4" s="57" t="s">
+      <c r="U4" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
       <c r="Y4" s="27"/>
       <c r="Z4" s="7" t="s">
         <v>17</v>
@@ -2003,11 +2003,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="19.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+    <row r="5" spans="1:27" ht="18.5" thickBot="1">
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2028,10 +2028,10 @@
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
       <c r="Q5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2064,8 +2064,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75">
-      <c r="A6" s="58" t="s">
+    <row r="6" spans="1:27">
+      <c r="A6" s="61" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -2091,7 +2091,7 @@
         <f>I6^3</f>
         <v>174.67687899999999</v>
       </c>
-      <c r="N6" s="60" t="s">
+      <c r="N6" s="63" t="s">
         <v>34</v>
       </c>
       <c r="O6" s="23">
@@ -2114,8 +2114,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75">
-      <c r="A7" s="59"/>
+    <row r="7" spans="1:27">
+      <c r="A7" s="62"/>
       <c r="B7" s="28" t="s">
         <v>32</v>
       </c>
@@ -2139,7 +2139,7 @@
         <f t="shared" ref="J7:J12" si="1">I7^3</f>
         <v>193.10055200000002</v>
       </c>
-      <c r="N7" s="55"/>
+      <c r="N7" s="59"/>
       <c r="O7" s="24">
         <v>1962</v>
       </c>
@@ -2160,8 +2160,8 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75">
-      <c r="A8" s="59"/>
+    <row r="8" spans="1:27">
+      <c r="A8" s="62"/>
       <c r="B8" s="28" t="s">
         <v>32</v>
       </c>
@@ -2185,7 +2185,7 @@
         <f t="shared" si="1"/>
         <v>183.25043199999999</v>
       </c>
-      <c r="N8" s="55"/>
+      <c r="N8" s="59"/>
       <c r="O8" s="24">
         <v>1962</v>
       </c>
@@ -2206,8 +2206,8 @@
         <v>5.12</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75">
-      <c r="A9" s="59"/>
+    <row r="9" spans="1:27">
+      <c r="A9" s="62"/>
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
@@ -2231,7 +2231,7 @@
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N9" s="55"/>
+      <c r="N9" s="59"/>
       <c r="O9" s="24">
         <v>1962</v>
       </c>
@@ -2252,8 +2252,8 @@
         <v>5.96</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75">
-      <c r="A10" s="59"/>
+    <row r="10" spans="1:27">
+      <c r="A10" s="62"/>
       <c r="B10" s="28" t="s">
         <v>32</v>
       </c>
@@ -2277,7 +2277,7 @@
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N10" s="55"/>
+      <c r="N10" s="59"/>
       <c r="O10" s="24">
         <v>1962</v>
       </c>
@@ -2299,7 +2299,7 @@
       </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="59" t="s">
         <v>38</v>
       </c>
       <c r="C11">
@@ -2322,7 +2322,7 @@
         <f t="shared" si="1"/>
         <v>186.16941100000003</v>
       </c>
-      <c r="N11" s="55"/>
+      <c r="N11" s="59"/>
       <c r="O11" s="24">
         <v>1962</v>
       </c>
@@ -2344,7 +2344,7 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="B12" s="55"/>
+      <c r="B12" s="59"/>
       <c r="C12">
         <v>1957</v>
       </c>
@@ -2365,7 +2365,7 @@
         <f t="shared" si="1"/>
         <v>188.52678690400001</v>
       </c>
-      <c r="N12" s="55"/>
+      <c r="N12" s="59"/>
       <c r="O12" s="24">
         <v>1962</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>9.65</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.75">
+    <row r="13" spans="1:27">
       <c r="A13" s="29" t="s">
         <v>40</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="F13">
         <v>29.65</v>
       </c>
-      <c r="N13" s="55"/>
+      <c r="N13" s="59"/>
       <c r="O13" s="24">
         <v>1962</v>
       </c>
@@ -2427,10 +2427,10 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="59" t="s">
         <v>43</v>
       </c>
       <c r="C14">
@@ -2474,8 +2474,8 @@
       </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="54"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15">
         <v>1960</v>
       </c>
@@ -2514,8 +2514,8 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="54"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16">
         <v>1960</v>
       </c>
@@ -2554,8 +2554,8 @@
       </c>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="54"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17">
         <v>1960</v>
       </c>
@@ -2577,9 +2577,9 @@
       </c>
       <c r="P17" s="24"/>
     </row>
-    <row r="18" spans="1:31" ht="15.75">
-      <c r="A18" s="54"/>
-      <c r="B18" s="55"/>
+    <row r="18" spans="1:31">
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18">
         <v>1960</v>
       </c>
@@ -7348,11 +7348,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="P3:P5"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="Z3:AA3"/>
@@ -7369,6 +7364,11 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="U3:X3"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="P3:P5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N6" r:id="rId1" xr:uid="{19CE446B-6698-4AD9-8C8B-B0EA1227F079}"/>
@@ -7396,17 +7396,17 @@
       <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="25.625" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="25.58203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="13.125" customWidth="1"/>
+    <col min="9" max="9" width="13.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" ht="15.75">
+    <row r="1" spans="1:9" s="21" customFormat="1">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -7419,18 +7419,18 @@
       <c r="H1" s="66"/>
       <c r="I1" s="66"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75">
+    <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1">
       <c r="A3" s="68" t="s">
@@ -7445,8 +7445,8 @@
       <c r="H3" s="68"/>
       <c r="I3" s="68"/>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="15.75">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:9" s="3" customFormat="1">
+      <c r="A4" s="64"/>
       <c r="B4" s="56" t="s">
         <v>5</v>
       </c>
@@ -7466,8 +7466,8 @@
       <c r="H4" s="56"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="61"/>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="17.149999999999999" customHeight="1">
+      <c r="A5" s="64"/>
       <c r="B5" s="56"/>
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
@@ -7477,19 +7477,19 @@
       <c r="F5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="57" t="s">
+      <c r="H5" s="60" t="s">
         <v>81</v>
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+    <row r="6" spans="1:9" s="11" customFormat="1" ht="17" thickBot="1">
+      <c r="A6" s="65"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
@@ -8879,34 +8879,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855DA3B9-8C38-4A4E-B8C1-649E45A85AE6}">
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
     <col min="2" max="2" width="12.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.75" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.75" style="18"/>
     <col min="12" max="12" width="12.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.375" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.75" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.875" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.125" style="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.08203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.08203125" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="21" customFormat="1" ht="15.75">
+    <row r="1" spans="1:18" s="21" customFormat="1">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -8919,7 +8919,7 @@
       <c r="H1" s="66"/>
       <c r="I1" s="66"/>
     </row>
-    <row r="2" spans="1:18" s="15" customFormat="1" ht="15.75">
+    <row r="2" spans="1:18" s="15" customFormat="1">
       <c r="A2" s="14"/>
       <c r="B2" s="69" t="s">
         <v>3</v>
@@ -8932,8 +8932,8 @@
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="19" customHeight="1">
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -8975,8 +8975,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -9000,11 +9000,11 @@
       <c r="P4" s="56"/>
       <c r="Q4" s="56"/>
     </row>
-    <row r="5" spans="1:18" s="17" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+    <row r="5" spans="1:18" s="17" customFormat="1" ht="18" thickBot="1">
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -9020,9 +9020,9 @@
       <c r="I5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -10710,25 +10710,25 @@
       <selection pane="bottomLeft" activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="21" customFormat="1" ht="15.75">
+    <row r="1" spans="1:18" s="21" customFormat="1">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -10741,7 +10741,7 @@
       <c r="H1" s="66"/>
       <c r="I1" s="66"/>
     </row>
-    <row r="2" spans="1:18" s="14" customFormat="1" ht="15.75">
+    <row r="2" spans="1:18" s="14" customFormat="1">
       <c r="B2" s="69" t="s">
         <v>3</v>
       </c>
@@ -10753,8 +10753,8 @@
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -10785,8 +10785,8 @@
       <c r="P3" s="56"/>
       <c r="Q3" s="56"/>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.149999999999999" customHeight="1">
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -10814,10 +10814,10 @@
       <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -10833,9 +10833,9 @@
       <c r="J5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -13401,12 +13401,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A5"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:K3"/>
@@ -13415,6 +13409,12 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13430,35 +13430,35 @@
       <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.08203125" style="18" customWidth="1"/>
     <col min="7" max="11" width="10.75" style="18"/>
     <col min="12" max="12" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.75" style="18"/>
-    <col min="14" max="14" width="12.625" style="18" customWidth="1"/>
+    <col min="14" max="14" width="12.58203125" style="18" customWidth="1"/>
     <col min="15" max="15" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1" ht="15.75">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:15" s="21" customFormat="1">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-    </row>
-    <row r="2" spans="1:15" s="15" customFormat="1" ht="15.75">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+    </row>
+    <row r="2" spans="1:15" s="15" customFormat="1">
       <c r="A2" s="14"/>
       <c r="B2" s="69" t="s">
         <v>3</v>
@@ -13468,8 +13468,8 @@
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
     </row>
-    <row r="3" spans="1:15" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="19" customHeight="1">
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -13494,19 +13494,19 @@
       <c r="M3" s="56"/>
       <c r="N3" s="56"/>
     </row>
-    <row r="4" spans="1:15" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:15" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="8"/>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
@@ -13515,10 +13515,10 @@
       <c r="N4" s="56"/>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -13534,8 +13534,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
       <c r="L5" s="10"/>
       <c r="M5" s="13"/>
       <c r="N5" s="16"/>
@@ -19613,7 +19613,7 @@
         <v>545.16</v>
       </c>
     </row>
-    <row r="345" spans="2:9" customFormat="1">
+    <row r="345" spans="2:9" customFormat="1" ht="28">
       <c r="B345" s="48" t="s">
         <v>129</v>
       </c>
@@ -20336,7 +20336,7 @@
         <v>143.96</v>
       </c>
     </row>
-    <row r="385" spans="2:7" customFormat="1" ht="29.25">
+    <row r="385" spans="2:7" customFormat="1" ht="29">
       <c r="B385" s="49" t="s">
         <v>130</v>
       </c>
@@ -21567,7 +21567,7 @@
         <v>-199.3</v>
       </c>
     </row>
-    <row r="448" spans="2:10" customFormat="1" ht="15.75">
+    <row r="448" spans="2:10" customFormat="1">
       <c r="C448" s="30">
         <v>1947</v>
       </c>
@@ -21589,7 +21589,7 @@
         <v>-191.3</v>
       </c>
     </row>
-    <row r="449" spans="3:10" customFormat="1" ht="15.75">
+    <row r="449" spans="3:10" customFormat="1">
       <c r="C449" s="30">
         <v>1947</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v>-187.2</v>
       </c>
     </row>
-    <row r="450" spans="3:10" customFormat="1" ht="15.75">
+    <row r="450" spans="3:10" customFormat="1">
       <c r="C450" s="30">
         <v>1947</v>
       </c>
@@ -21633,7 +21633,7 @@
         <v>-182.9</v>
       </c>
     </row>
-    <row r="451" spans="3:10" customFormat="1" ht="15.75">
+    <row r="451" spans="3:10" customFormat="1">
       <c r="C451" s="30">
         <v>1947</v>
       </c>
@@ -21655,7 +21655,7 @@
         <v>-178.4</v>
       </c>
     </row>
-    <row r="452" spans="3:10" customFormat="1" ht="15.75">
+    <row r="452" spans="3:10" customFormat="1">
       <c r="C452" s="30">
         <v>1947</v>
       </c>
@@ -21677,7 +21677,7 @@
         <v>-175.7</v>
       </c>
     </row>
-    <row r="453" spans="3:10" customFormat="1" ht="15.75">
+    <row r="453" spans="3:10" customFormat="1">
       <c r="C453" s="30">
         <v>1947</v>
       </c>
@@ -21699,7 +21699,7 @@
         <v>-171.8</v>
       </c>
     </row>
-    <row r="454" spans="3:10" customFormat="1" ht="15.75">
+    <row r="454" spans="3:10" customFormat="1">
       <c r="C454" s="30">
         <v>1947</v>
       </c>
@@ -21721,7 +21721,7 @@
         <v>-165.9</v>
       </c>
     </row>
-    <row r="455" spans="3:10" customFormat="1" ht="15.75">
+    <row r="455" spans="3:10" customFormat="1">
       <c r="C455" s="30">
         <v>1947</v>
       </c>
@@ -21743,7 +21743,7 @@
         <v>-159</v>
       </c>
     </row>
-    <row r="456" spans="3:10" customFormat="1" ht="15.75">
+    <row r="456" spans="3:10" customFormat="1">
       <c r="C456" s="30">
         <v>1947</v>
       </c>
@@ -22117,40 +22117,40 @@
   <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="H72" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="5" topLeftCell="A72" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
     <col min="6" max="6" width="12" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
     <col min="8" max="12" width="10.75" style="18"/>
     <col min="13" max="13" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.75" style="18"/>
-    <col min="15" max="15" width="12.625" style="18" customWidth="1"/>
+    <col min="15" max="15" width="12.58203125" style="18" customWidth="1"/>
     <col min="16" max="16" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="21" customFormat="1" ht="15.75">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:16" s="21" customFormat="1">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-    </row>
-    <row r="2" spans="1:16" s="15" customFormat="1" ht="15.75">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+    </row>
+    <row r="2" spans="1:16" s="15" customFormat="1">
       <c r="A2" s="14"/>
       <c r="B2" s="69" t="s">
         <v>3</v>
@@ -22160,8 +22160,8 @@
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="19" customHeight="1">
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -22191,19 +22191,19 @@
       <c r="N3" s="56"/>
       <c r="O3" s="56"/>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:16" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="8"/>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
@@ -22213,10 +22213,10 @@
       <c r="O4" s="56"/>
     </row>
     <row r="5" spans="1:16" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -22232,8 +22232,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
       <c r="L5" s="10" t="s">
         <v>28</v>
       </c>
@@ -23861,32 +23861,32 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5FF47D-C774-6B45-AE66-2A4B51DD47F5}">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="C20" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="5" topLeftCell="A20" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="17.125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="17.08203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="21" customFormat="1" ht="15.75">
+    <row r="1" spans="1:18" s="21" customFormat="1">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -23899,7 +23899,7 @@
       <c r="H1" s="66"/>
       <c r="I1" s="66"/>
     </row>
-    <row r="2" spans="1:18" s="15" customFormat="1" ht="15.75">
+    <row r="2" spans="1:18" s="15" customFormat="1">
       <c r="A2" s="14"/>
       <c r="B2" s="69" t="s">
         <v>3</v>
@@ -23912,8 +23912,8 @@
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="19" customHeight="1">
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -23939,8 +23939,8 @@
       <c r="P3" s="56"/>
       <c r="Q3" s="56"/>
     </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -23967,10 +23967,10 @@
       <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -23986,15 +23986,15 @@
       <c r="I5" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="O5" s="10"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18" ht="15.75">
+    <row r="6" spans="1:18">
       <c r="B6" s="19"/>
       <c r="C6" s="36">
         <v>1978</v>
@@ -24009,7 +24009,7 @@
         <v>10.993</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75">
+    <row r="7" spans="1:18">
       <c r="B7" s="19"/>
       <c r="C7" s="36">
         <v>1978</v>
@@ -24024,7 +24024,7 @@
         <v>10.988</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75">
+    <row r="8" spans="1:18">
       <c r="B8" s="19"/>
       <c r="C8" s="36">
         <v>1978</v>
@@ -24039,7 +24039,7 @@
         <v>10.981999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75">
+    <row r="9" spans="1:18">
       <c r="B9" s="19"/>
       <c r="C9" s="36">
         <v>1978</v>
@@ -24054,7 +24054,7 @@
         <v>10.976000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75">
+    <row r="10" spans="1:18">
       <c r="B10" s="19"/>
       <c r="C10" s="36">
         <v>1978</v>
@@ -24069,7 +24069,7 @@
         <v>10.97</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75">
+    <row r="11" spans="1:18">
       <c r="B11" s="19"/>
       <c r="C11" s="36">
         <v>1978</v>
@@ -24084,7 +24084,7 @@
         <v>10.962999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75">
+    <row r="12" spans="1:18">
       <c r="B12" s="19"/>
       <c r="C12" s="36">
         <v>1978</v>
@@ -24099,7 +24099,7 @@
         <v>10.957000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75">
+    <row r="13" spans="1:18">
       <c r="B13" s="19"/>
       <c r="C13" s="36">
         <v>1978</v>
@@ -24114,7 +24114,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75">
+    <row r="14" spans="1:18">
       <c r="B14" s="19"/>
       <c r="C14" s="36">
         <v>1978</v>
@@ -24129,7 +24129,7 @@
         <v>10.943</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75">
+    <row r="15" spans="1:18">
       <c r="B15" s="19"/>
       <c r="C15" s="36">
         <v>1978</v>
@@ -24144,7 +24144,7 @@
         <v>10.936</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75">
+    <row r="16" spans="1:18">
       <c r="B16" s="19"/>
       <c r="C16" s="36">
         <v>1978</v>
@@ -24159,7 +24159,7 @@
         <v>10.928000000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.75">
+    <row r="17" spans="2:6">
       <c r="B17" s="19"/>
       <c r="C17" s="36">
         <v>1978</v>
@@ -24174,7 +24174,7 @@
         <v>10.92</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="15.75">
+    <row r="18" spans="2:6">
       <c r="B18" s="19"/>
       <c r="C18" s="36">
         <v>1978</v>
@@ -24189,7 +24189,7 @@
         <v>10.913</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="15.75">
+    <row r="19" spans="2:6">
       <c r="C19" s="36">
         <v>1978</v>
       </c>
@@ -24203,7 +24203,7 @@
         <v>10.904999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15.75">
+    <row r="20" spans="2:6">
       <c r="C20" s="36">
         <v>1978</v>
       </c>
@@ -24217,7 +24217,7 @@
         <v>10.896000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="15.75">
+    <row r="21" spans="2:6">
       <c r="C21" s="36">
         <v>1978</v>
       </c>
@@ -24231,7 +24231,7 @@
         <v>10.888</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="15.75">
+    <row r="22" spans="2:6">
       <c r="C22" s="36">
         <v>1978</v>
       </c>
@@ -24245,7 +24245,7 @@
         <v>10.879</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="15.75">
+    <row r="23" spans="2:6">
       <c r="C23" s="36">
         <v>1978</v>
       </c>
@@ -24259,7 +24259,7 @@
         <v>10.87</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="15.75">
+    <row r="24" spans="2:6">
       <c r="C24" s="36">
         <v>1978</v>
       </c>
@@ -24273,7 +24273,7 @@
         <v>10.86</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15.75">
+    <row r="25" spans="2:6">
       <c r="C25" s="36">
         <v>1978</v>
       </c>
@@ -24287,7 +24287,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="15.75">
+    <row r="26" spans="2:6">
       <c r="C26" s="36">
         <v>1978</v>
       </c>
@@ -24301,7 +24301,7 @@
         <v>10.84</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="15.75">
+    <row r="27" spans="2:6">
       <c r="C27" s="36">
         <v>1978</v>
       </c>
@@ -24315,7 +24315,7 @@
         <v>10.83</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="15.75">
+    <row r="28" spans="2:6">
       <c r="C28" s="36">
         <v>1978</v>
       </c>
@@ -24329,7 +24329,7 @@
         <v>10.819000000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="15.75">
+    <row r="29" spans="2:6">
       <c r="C29" s="36">
         <v>1978</v>
       </c>
@@ -24343,7 +24343,7 @@
         <v>10.808</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="15.75">
+    <row r="30" spans="2:6">
       <c r="C30" s="36">
         <v>1978</v>
       </c>
@@ -24357,7 +24357,7 @@
         <v>10.797000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="15.75">
+    <row r="31" spans="2:6">
       <c r="C31" s="36">
         <v>1978</v>
       </c>
@@ -24371,7 +24371,7 @@
         <v>10.785</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="15.75">
+    <row r="32" spans="2:6">
       <c r="C32" s="36">
         <v>1978</v>
       </c>
@@ -24385,7 +24385,7 @@
         <v>10.773</v>
       </c>
     </row>
-    <row r="33" spans="3:6" ht="15.75">
+    <row r="33" spans="3:6">
       <c r="C33" s="36">
         <v>1978</v>
       </c>
@@ -24399,21 +24399,8 @@
         <v>10.760999999999999</v>
       </c>
     </row>
-    <row r="34" spans="3:6" ht="15.75"/>
-    <row r="35" spans="3:6" ht="15.75"/>
-    <row r="36" spans="3:6" ht="15.75"/>
-    <row r="37" spans="3:6" ht="15.75"/>
-    <row r="38" spans="3:6" ht="15.75"/>
-    <row r="39" spans="3:6" ht="15.75"/>
-    <row r="40" spans="3:6" ht="15.75"/>
-    <row r="41" spans="3:6" ht="15.75"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B2:I2"/>
@@ -24421,6 +24408,11 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -24436,25 +24428,25 @@
       <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="21" customFormat="1" ht="15.75">
+    <row r="1" spans="1:18" s="21" customFormat="1">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -24467,7 +24459,7 @@
       <c r="H1" s="66"/>
       <c r="I1" s="66"/>
     </row>
-    <row r="2" spans="1:18" s="14" customFormat="1" ht="15.75">
+    <row r="2" spans="1:18" s="14" customFormat="1">
       <c r="B2" s="69" t="s">
         <v>3</v>
       </c>
@@ -24479,8 +24471,8 @@
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -24515,8 +24507,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.149999999999999" customHeight="1">
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -24537,11 +24529,11 @@
       <c r="P4" s="56"/>
       <c r="Q4" s="56"/>
     </row>
-    <row r="5" spans="1:18" s="10" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+    <row r="5" spans="1:18" s="10" customFormat="1" ht="18" thickBot="1">
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24557,9 +24549,9 @@
       <c r="I5" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24760,17 +24752,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
trying to play with weightings
</commit_message>
<xml_diff>
--- a/data/MASTER Krypton Literature Review.xlsx
+++ b/data/MASTER Krypton Literature Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23059859_student_uwa_edu_au/Documents/UWA/05. Year 5/Semester 1/GENG5511 MPE Engineering Research Project/Project/Research_Project/GENG5511_Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EA16B5B-F567-4016-80B1-C299924FB7FE}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C890D860-6718-4809-9234-89A2C8CE8454}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell Volume " sheetId="1" r:id="rId1"/>
@@ -1394,23 +1394,14 @@
     <xf numFmtId="4" fontId="21" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1429,6 +1420,15 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1784,17 +1784,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F513A9-1C82-3E45-A361-2C7180831D5E}">
   <dimension ref="A1:AE136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="6.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
@@ -1804,14 +1804,14 @@
     <col min="11" max="11" width="12.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.08203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.75" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.25" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.58203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.5" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="4.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.5" bestFit="1" customWidth="1"/>
@@ -1819,18 +1819,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
       <c r="K1" s="26" t="s">
         <v>1</v>
       </c>
@@ -1855,17 +1855,17 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="5"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
       <c r="K2" s="2">
         <f>6.02214076*10^23</f>
         <v>6.0221407599999999E+23</v>
@@ -1890,7 +1890,7 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="61" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="56" t="s">
@@ -1918,7 +1918,7 @@
       <c r="J3" s="56"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="64" t="s">
+      <c r="M3" s="61" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="56" t="s">
@@ -1952,8 +1952,8 @@
       </c>
       <c r="AA3" s="56"/>
     </row>
-    <row r="4" spans="1:27" ht="16.5">
-      <c r="A4" s="64"/>
+    <row r="4" spans="1:27" ht="18">
+      <c r="A4" s="61"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -1963,10 +1963,10 @@
       <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="60"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="7" t="s">
         <v>17</v>
       </c>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="64"/>
+      <c r="M4" s="61"/>
       <c r="N4" s="56"/>
       <c r="O4" s="56"/>
       <c r="P4" s="56"/>
@@ -1989,12 +1989,12 @@
         <v>16</v>
       </c>
       <c r="T4" s="7"/>
-      <c r="U4" s="60" t="s">
+      <c r="U4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="60"/>
-      <c r="W4" s="60"/>
-      <c r="X4" s="60"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
       <c r="Y4" s="27"/>
       <c r="Z4" s="7" t="s">
         <v>17</v>
@@ -2003,11 +2003,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="18.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+    <row r="5" spans="1:27" ht="18.75" thickBot="1">
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2028,10 +2028,10 @@
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
       <c r="Q5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2065,7 +2065,7 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="58" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -2091,7 +2091,7 @@
         <f>I6^3</f>
         <v>174.67687899999999</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="60" t="s">
         <v>34</v>
       </c>
       <c r="O6" s="23">
@@ -2115,7 +2115,7 @@
       </c>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="62"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="28" t="s">
         <v>32</v>
       </c>
@@ -2139,7 +2139,7 @@
         <f t="shared" ref="J7:J12" si="1">I7^3</f>
         <v>193.10055200000002</v>
       </c>
-      <c r="N7" s="59"/>
+      <c r="N7" s="55"/>
       <c r="O7" s="24">
         <v>1962</v>
       </c>
@@ -2161,7 +2161,7 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="62"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="28" t="s">
         <v>32</v>
       </c>
@@ -2185,7 +2185,7 @@
         <f t="shared" si="1"/>
         <v>183.25043199999999</v>
       </c>
-      <c r="N8" s="59"/>
+      <c r="N8" s="55"/>
       <c r="O8" s="24">
         <v>1962</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="62"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
@@ -2231,7 +2231,7 @@
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N9" s="59"/>
+      <c r="N9" s="55"/>
       <c r="O9" s="24">
         <v>1962</v>
       </c>
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="62"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="28" t="s">
         <v>32</v>
       </c>
@@ -2277,7 +2277,7 @@
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N10" s="59"/>
+      <c r="N10" s="55"/>
       <c r="O10" s="24">
         <v>1962</v>
       </c>
@@ -2299,7 +2299,7 @@
       </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C11">
@@ -2322,7 +2322,7 @@
         <f t="shared" si="1"/>
         <v>186.16941100000003</v>
       </c>
-      <c r="N11" s="59"/>
+      <c r="N11" s="55"/>
       <c r="O11" s="24">
         <v>1962</v>
       </c>
@@ -2344,7 +2344,7 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="B12" s="59"/>
+      <c r="B12" s="55"/>
       <c r="C12">
         <v>1957</v>
       </c>
@@ -2365,7 +2365,7 @@
         <f t="shared" si="1"/>
         <v>188.52678690400001</v>
       </c>
-      <c r="N12" s="59"/>
+      <c r="N12" s="55"/>
       <c r="O12" s="24">
         <v>1962</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="F13">
         <v>29.65</v>
       </c>
-      <c r="N13" s="59"/>
+      <c r="N13" s="55"/>
       <c r="O13" s="24">
         <v>1962</v>
       </c>
@@ -2427,10 +2427,10 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="55" t="s">
         <v>43</v>
       </c>
       <c r="C14">
@@ -2474,8 +2474,8 @@
       </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="55"/>
       <c r="C15">
         <v>1960</v>
       </c>
@@ -2514,8 +2514,8 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="58"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="55"/>
       <c r="C16">
         <v>1960</v>
       </c>
@@ -2554,8 +2554,8 @@
       </c>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="58"/>
-      <c r="B17" s="59"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="55"/>
       <c r="C17">
         <v>1960</v>
       </c>
@@ -2578,8 +2578,8 @@
       <c r="P17" s="24"/>
     </row>
     <row r="18" spans="1:31">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="55"/>
       <c r="C18">
         <v>1960</v>
       </c>
@@ -7348,6 +7348,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="P3:P5"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="Z3:AA3"/>
@@ -7364,11 +7369,6 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="U3:X3"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="P3:P5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N6" r:id="rId1" xr:uid="{19CE446B-6698-4AD9-8C8B-B0EA1227F079}"/>
@@ -7391,19 +7391,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34482523-6132-7E48-BEBF-BE687D0AD34C}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView zoomScale="69" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A97" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="25.58203125" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="13.08203125" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="21" customFormat="1">
@@ -7421,16 +7421,16 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1">
       <c r="A3" s="68" t="s">
@@ -7446,7 +7446,7 @@
       <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1">
-      <c r="A4" s="64"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="56" t="s">
         <v>5</v>
       </c>
@@ -7466,8 +7466,8 @@
       <c r="H4" s="56"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A5" s="64"/>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="61"/>
       <c r="B5" s="56"/>
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
@@ -7477,19 +7477,19 @@
       <c r="F5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="60" t="s">
+      <c r="H5" s="57" t="s">
         <v>81</v>
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" ht="17" thickBot="1">
-      <c r="A6" s="65"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+    <row r="6" spans="1:9" s="11" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
@@ -8884,25 +8884,25 @@
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
     <col min="2" max="2" width="12.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.375" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.75" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.875" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.75" style="18"/>
     <col min="12" max="12" width="12.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.375" style="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.75" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.875" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.08203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.08203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.125" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
@@ -8932,8 +8932,8 @@
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="64"/>
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="61"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -8975,8 +8975,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="64"/>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="61"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -9000,11 +9000,11 @@
       <c r="P4" s="56"/>
       <c r="Q4" s="56"/>
     </row>
-    <row r="5" spans="1:18" s="17" customFormat="1" ht="18" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+    <row r="5" spans="1:18" s="17" customFormat="1" ht="19.5" thickBot="1">
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -9020,9 +9020,9 @@
       <c r="I5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -10706,24 +10706,24 @@
   <dimension ref="A1:R152"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A36" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I138" sqref="I138"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
@@ -10753,8 +10753,8 @@
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="64"/>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="61"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -10785,8 +10785,8 @@
       <c r="P3" s="56"/>
       <c r="Q3" s="56"/>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="64"/>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="61"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -10814,10 +10814,10 @@
       <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -10833,9 +10833,9 @@
       <c r="J5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -11548,7 +11548,7 @@
         <v>0.54520000000000002</v>
       </c>
       <c r="F44" s="37">
-        <f t="shared" si="0"/>
+        <f>H44/1000</f>
         <v>8.2649999999999998E-4</v>
       </c>
       <c r="H44" s="42">
@@ -13401,6 +13401,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:K3"/>
@@ -13409,12 +13415,6 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13430,33 +13430,33 @@
       <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.08203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.125" style="18" customWidth="1"/>
     <col min="7" max="11" width="10.75" style="18"/>
     <col min="12" max="12" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.75" style="18"/>
-    <col min="14" max="14" width="12.58203125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="12.625" style="18" customWidth="1"/>
     <col min="15" max="15" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1">
       <c r="A2" s="14"/>
@@ -13468,8 +13468,8 @@
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
     </row>
-    <row r="3" spans="1:15" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="64"/>
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="61"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -13494,19 +13494,19 @@
       <c r="M3" s="56"/>
       <c r="N3" s="56"/>
     </row>
-    <row r="4" spans="1:15" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="64"/>
+    <row r="4" spans="1:15" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="61"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="8"/>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
@@ -13515,10 +13515,10 @@
       <c r="N4" s="56"/>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -13534,8 +13534,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
       <c r="L5" s="10"/>
       <c r="M5" s="13"/>
       <c r="N5" s="16"/>
@@ -19613,7 +19613,7 @@
         <v>545.16</v>
       </c>
     </row>
-    <row r="345" spans="2:9" customFormat="1" ht="28">
+    <row r="345" spans="2:9" customFormat="1" ht="28.5">
       <c r="B345" s="48" t="s">
         <v>129</v>
       </c>
@@ -20336,7 +20336,7 @@
         <v>143.96</v>
       </c>
     </row>
-    <row r="385" spans="2:7" customFormat="1" ht="29">
+    <row r="385" spans="2:7" customFormat="1" ht="30">
       <c r="B385" s="49" t="s">
         <v>130</v>
       </c>
@@ -22121,34 +22121,34 @@
       <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
     <col min="6" max="6" width="12" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
     <col min="8" max="12" width="10.75" style="18"/>
     <col min="13" max="13" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.75" style="18"/>
-    <col min="15" max="15" width="12.58203125" style="18" customWidth="1"/>
+    <col min="15" max="15" width="12.625" style="18" customWidth="1"/>
     <col min="16" max="16" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="21" customFormat="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
     </row>
     <row r="2" spans="1:16" s="15" customFormat="1">
       <c r="A2" s="14"/>
@@ -22160,8 +22160,8 @@
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="64"/>
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="61"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -22191,19 +22191,19 @@
       <c r="N3" s="56"/>
       <c r="O3" s="56"/>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="64"/>
+    <row r="4" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="61"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="8"/>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
@@ -22213,10 +22213,10 @@
       <c r="O4" s="56"/>
     </row>
     <row r="5" spans="1:16" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -22232,8 +22232,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
       <c r="L5" s="10" t="s">
         <v>28</v>
       </c>
@@ -23864,24 +23864,24 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A20" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="17.08203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="17.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
@@ -23912,8 +23912,8 @@
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="64"/>
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="61"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -23939,8 +23939,8 @@
       <c r="P3" s="56"/>
       <c r="Q3" s="56"/>
     </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="64"/>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="61"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -23967,10 +23967,10 @@
       <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -23986,9 +23986,9 @@
       <c r="I5" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="O5" s="10"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
@@ -24401,6 +24401,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B2:I2"/>
@@ -24408,11 +24413,6 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -24428,20 +24428,20 @@
       <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
@@ -24471,8 +24471,8 @@
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="64"/>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="61"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -24507,8 +24507,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="64"/>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="61"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -24529,11 +24529,11 @@
       <c r="P4" s="56"/>
       <c r="Q4" s="56"/>
     </row>
-    <row r="5" spans="1:18" s="10" customFormat="1" ht="18" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+    <row r="5" spans="1:18" s="10" customFormat="1" ht="19.5" thickBot="1">
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24549,9 +24549,9 @@
       <c r="I5" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24752,17 +24752,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
working on fitting xenon
</commit_message>
<xml_diff>
--- a/data/MASTER Krypton Literature Review.xlsx
+++ b/data/MASTER Krypton Literature Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23059859_student_uwa_edu_au/Documents/UWA/05. Year 5/Semester 1/GENG5511 MPE Engineering Research Project/Project/Research_Project/GENG5511_Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C890D860-6718-4809-9234-89A2C8CE8454}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2645D7EC-3D01-477E-9FE3-DF6B6504B65D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell Volume " sheetId="1" r:id="rId1"/>
@@ -1164,7 +1164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1210,6 +1210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1273,7 +1279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1394,14 +1400,23 @@
     <xf numFmtId="4" fontId="21" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1421,15 +1436,6 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1442,6 +1448,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1784,9 +1791,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F513A9-1C82-3E45-A361-2C7180831D5E}">
   <dimension ref="A1:AE136"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.875" defaultRowHeight="15.75"/>
@@ -1819,18 +1826,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="26" t="s">
         <v>1</v>
       </c>
@@ -1855,17 +1862,17 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="5"/>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="2">
         <f>6.02214076*10^23</f>
         <v>6.0221407599999999E+23</v>
@@ -1890,7 +1897,7 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="64" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="56" t="s">
@@ -1918,7 +1925,7 @@
       <c r="J3" s="56"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="61" t="s">
+      <c r="M3" s="64" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="56" t="s">
@@ -1953,7 +1960,7 @@
       <c r="AA3" s="56"/>
     </row>
     <row r="4" spans="1:27" ht="18">
-      <c r="A4" s="61"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -1963,10 +1970,10 @@
       <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="57"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="7" t="s">
         <v>17</v>
       </c>
@@ -1975,7 +1982,7 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="61"/>
+      <c r="M4" s="64"/>
       <c r="N4" s="56"/>
       <c r="O4" s="56"/>
       <c r="P4" s="56"/>
@@ -1989,12 +1996,12 @@
         <v>16</v>
       </c>
       <c r="T4" s="7"/>
-      <c r="U4" s="57" t="s">
+      <c r="U4" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
       <c r="Y4" s="27"/>
       <c r="Z4" s="7" t="s">
         <v>17</v>
@@ -2004,10 +2011,10 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="18.75" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2028,10 +2035,10 @@
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
       <c r="Q5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2065,33 +2072,35 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="61" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="70">
         <v>1930</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="70">
         <v>20</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="70">
         <f>(J6*10^-30)*$K$2*(1*10^6)/4</f>
         <v>26.298218821387195</v>
       </c>
-      <c r="I6">
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70">
         <v>5.59</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="70">
         <f>I6^3</f>
         <v>174.67687899999999</v>
       </c>
-      <c r="N6" s="60" t="s">
+      <c r="N6" s="63" t="s">
         <v>34</v>
       </c>
       <c r="O6" s="23">
@@ -2115,31 +2124,33 @@
       </c>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="59"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="70">
         <v>1930</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="70">
         <v>78</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="70">
         <f t="shared" ref="F7:F12" si="0">(J7*10^-30)*$K$2*(1*10^6)/4</f>
         <v>29.07196762444249</v>
       </c>
-      <c r="I7">
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70">
         <v>5.78</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="70">
         <f t="shared" ref="J7:J12" si="1">I7^3</f>
         <v>193.10055200000002</v>
       </c>
-      <c r="N7" s="55"/>
+      <c r="N7" s="59"/>
       <c r="O7" s="24">
         <v>1962</v>
       </c>
@@ -2161,31 +2172,33 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="59"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="70">
         <v>1932</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="70">
         <v>82</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="70">
         <f t="shared" si="0"/>
         <v>27.588997395870205</v>
       </c>
-      <c r="I8">
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70">
         <v>5.68</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="70">
         <f t="shared" si="1"/>
         <v>183.25043199999999</v>
       </c>
-      <c r="N8" s="55"/>
+      <c r="N8" s="59"/>
       <c r="O8" s="24">
         <v>1962</v>
       </c>
@@ -2207,31 +2220,33 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="59"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="70">
         <v>1932</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="70">
         <v>89</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="70">
         <f t="shared" si="0"/>
         <v>27.734970625161669</v>
       </c>
-      <c r="I9">
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70">
         <v>5.69</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="70">
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N9" s="55"/>
+      <c r="N9" s="59"/>
       <c r="O9" s="24">
         <v>1962</v>
       </c>
@@ -2253,31 +2268,33 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="59"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="70">
         <v>1932</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="70">
         <v>92</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="70">
         <f t="shared" si="0"/>
         <v>27.734970625161669</v>
       </c>
-      <c r="I10">
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70">
         <v>5.69</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="70">
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N10" s="55"/>
+      <c r="N10" s="59"/>
       <c r="O10" s="24">
         <v>1962</v>
       </c>
@@ -2299,7 +2316,7 @@
       </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="59" t="s">
         <v>38</v>
       </c>
       <c r="C11">
@@ -2322,7 +2339,7 @@
         <f t="shared" si="1"/>
         <v>186.16941100000003</v>
       </c>
-      <c r="N11" s="55"/>
+      <c r="N11" s="59"/>
       <c r="O11" s="24">
         <v>1962</v>
       </c>
@@ -2344,7 +2361,7 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="B12" s="55"/>
+      <c r="B12" s="59"/>
       <c r="C12">
         <v>1957</v>
       </c>
@@ -2365,7 +2382,7 @@
         <f t="shared" si="1"/>
         <v>188.52678690400001</v>
       </c>
-      <c r="N12" s="55"/>
+      <c r="N12" s="59"/>
       <c r="O12" s="24">
         <v>1962</v>
       </c>
@@ -2405,7 +2422,7 @@
       <c r="F13">
         <v>29.65</v>
       </c>
-      <c r="N13" s="55"/>
+      <c r="N13" s="59"/>
       <c r="O13" s="24">
         <v>1962</v>
       </c>
@@ -2427,10 +2444,10 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="59" t="s">
         <v>43</v>
       </c>
       <c r="C14">
@@ -2474,8 +2491,8 @@
       </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="54"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15">
         <v>1960</v>
       </c>
@@ -2514,8 +2531,8 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="54"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16">
         <v>1960</v>
       </c>
@@ -2554,8 +2571,8 @@
       </c>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="54"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17">
         <v>1960</v>
       </c>
@@ -2578,8 +2595,8 @@
       <c r="P17" s="24"/>
     </row>
     <row r="18" spans="1:31">
-      <c r="A18" s="54"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18">
         <v>1960</v>
       </c>
@@ -7348,11 +7365,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="P3:P5"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="Z3:AA3"/>
@@ -7369,6 +7381,11 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="U3:X3"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="P3:P5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N6" r:id="rId1" xr:uid="{19CE446B-6698-4AD9-8C8B-B0EA1227F079}"/>
@@ -7391,7 +7408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34482523-6132-7E48-BEBF-BE687D0AD34C}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+    <sheetView zoomScale="69" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
@@ -7421,16 +7438,16 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1">
       <c r="A3" s="68" t="s">
@@ -7446,7 +7463,7 @@
       <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1">
-      <c r="A4" s="61"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="56" t="s">
         <v>5</v>
       </c>
@@ -7467,7 +7484,7 @@
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="61"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="56"/>
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
@@ -7477,19 +7494,19 @@
       <c r="F5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="57" t="s">
+      <c r="H5" s="60" t="s">
         <v>81</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" s="11" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
@@ -8933,7 +8950,7 @@
       <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -8976,7 +8993,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -9001,10 +9018,10 @@
       <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -9020,9 +9037,9 @@
       <c r="I5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -10754,7 +10771,7 @@
       <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -10786,7 +10803,7 @@
       <c r="Q3" s="56"/>
     </row>
     <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -10814,10 +10831,10 @@
       <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -10833,9 +10850,9 @@
       <c r="J5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -13401,12 +13418,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A5"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:K3"/>
@@ -13415,6 +13426,12 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13446,17 +13463,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1">
       <c r="A2" s="14"/>
@@ -13469,7 +13486,7 @@
       <c r="F2" s="69"/>
     </row>
     <row r="3" spans="1:15" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -13495,18 +13512,18 @@
       <c r="N3" s="56"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="8"/>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
@@ -13515,10 +13532,10 @@
       <c r="N4" s="56"/>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -13534,8 +13551,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
       <c r="L5" s="10"/>
       <c r="M5" s="13"/>
       <c r="N5" s="16"/>
@@ -22138,17 +22155,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="21" customFormat="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:16" s="15" customFormat="1">
       <c r="A2" s="14"/>
@@ -22161,7 +22178,7 @@
       <c r="F2" s="69"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -22192,18 +22209,18 @@
       <c r="O3" s="56"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="8"/>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
@@ -22213,10 +22230,10 @@
       <c r="O4" s="56"/>
     </row>
     <row r="5" spans="1:16" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -22232,8 +22249,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
       <c r="L5" s="10" t="s">
         <v>28</v>
       </c>
@@ -23913,7 +23930,7 @@
       <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -23940,7 +23957,7 @@
       <c r="Q3" s="56"/>
     </row>
     <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -23967,10 +23984,10 @@
       <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -23986,9 +24003,9 @@
       <c r="I5" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="O5" s="10"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
@@ -24401,11 +24418,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B2:I2"/>
@@ -24413,6 +24425,11 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -24472,7 +24489,7 @@
       <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="61"/>
+      <c r="A3" s="64"/>
       <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
@@ -24508,7 +24525,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="61"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -24530,10 +24547,10 @@
       <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24549,9 +24566,9 @@
       <c r="I5" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24752,17 +24769,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
xenon fitted without enthalpy
</commit_message>
<xml_diff>
--- a/data/MASTER Krypton Literature Review.xlsx
+++ b/data/MASTER Krypton Literature Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23059859_student_uwa_edu_au/Documents/UWA/05. Year 5/Semester 1/GENG5511 MPE Engineering Research Project/Project/Research_Project/GENG5511_Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2645D7EC-3D01-477E-9FE3-DF6B6504B65D}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02B01D87-0D55-426E-B4EC-4F6580E07601}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell Volume " sheetId="1" r:id="rId1"/>
@@ -1400,23 +1400,15 @@
     <xf numFmtId="4" fontId="21" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1436,6 +1428,15 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1448,7 +1449,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1470,6 +1470,1346 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Cell Volume '!$E$6:$E$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>115.95</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>115.78</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>114.7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>109.88</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>99.775000000000006</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>89.662999999999997</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>79.551000000000002</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>69.438000000000002</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>59.326000000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>49.213000000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>39.774999999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>29.663</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>19.550999999999998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9.4380000000000006</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.7190000000000003</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.3480000000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Cell Volume '!$F$6:$F$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>26.298218821387195</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.07196762444249</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.588997395870205</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.734970625161669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.734970625161669</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.02845995620731</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.383371194160311</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.224821312540612</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.565131578947369</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.044846050870149</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.6390977443609</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.965779467680612</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.092790171354672</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.092790171354672</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.101552393272961</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.136658031088082</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27.19831223628692</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.269118125610152</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.358145608880182</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>27.556067083196318</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>27.793698175787728</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27.08212572064819</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27.097000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>27.099</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27.103000000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.111999999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.145</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27.202000000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>27.273</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>27.356999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>27.452000000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>27.552</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>27.658999999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>27.771000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>27.888000000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>28.012</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>28.141999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>28.279</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>28.420999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>28.571000000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>28.727</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>28.893000000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>29.067</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>29.245999999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>29.440999999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>29.654</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>29.884</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>29.922999999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>29.062999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>29.244</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>29.439</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>29.651</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>29.881</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>29.7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>28.727459718889271</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>28.895862068965517</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>29.076335877862594</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>29.259078212290504</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>29.464838255977497</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>29.705069124423961</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>29.959957096889525</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>29.756284349482854</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>29.344420954173533</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28.981526034136749</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>28.666457860136831</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>28.368523746582962</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>28.087405173417157</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>27.808149929492533</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>27.588997395870205</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>27.370999306631575</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>27.197429986464631</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>27.12532655113036</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>27.096520897023467</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>27.096520897023467</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>27.094000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD9C-4E0C-8FA0-F8E5DA86AAF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2069486895"/>
+        <c:axId val="2069489295"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2069486895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2069489295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2069489295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2069486895"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>496660</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>111579</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>292553</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>201386</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71BCF3A6-5DFF-07B2-7B9E-9DB2D8D10452}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1791,9 +3131,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F513A9-1C82-3E45-A361-2C7180831D5E}">
   <dimension ref="A1:AE136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AK68" sqref="AK68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.875" defaultRowHeight="15.75"/>
@@ -1826,18 +3166,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
       <c r="K1" s="26" t="s">
         <v>1</v>
       </c>
@@ -1862,17 +3202,17 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="5"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
       <c r="K2" s="2">
         <f>6.02214076*10^23</f>
         <v>6.0221407599999999E+23</v>
@@ -1897,16 +3237,16 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -1915,26 +3255,26 @@
       <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56" t="s">
+      <c r="H3" s="57"/>
+      <c r="I3" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="56"/>
+      <c r="J3" s="57"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="64" t="s">
+      <c r="M3" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="N3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="56" t="s">
+      <c r="P3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -1947,33 +3287,33 @@
         <v>10</v>
       </c>
       <c r="T3" s="6"/>
-      <c r="U3" s="56" t="s">
+      <c r="U3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
       <c r="Y3" s="8"/>
-      <c r="Z3" s="56" t="s">
+      <c r="Z3" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="56"/>
+      <c r="AA3" s="57"/>
     </row>
     <row r="4" spans="1:27" ht="18">
-      <c r="A4" s="64"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="60"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="7" t="s">
         <v>17</v>
       </c>
@@ -1982,10 +3322,10 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
       <c r="Q4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1996,12 +3336,12 @@
         <v>16</v>
       </c>
       <c r="T4" s="7"/>
-      <c r="U4" s="60" t="s">
+      <c r="U4" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="60"/>
-      <c r="W4" s="60"/>
-      <c r="X4" s="60"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
       <c r="Y4" s="27"/>
       <c r="Z4" s="7" t="s">
         <v>17</v>
@@ -2011,10 +3351,10 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="18.75" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2035,10 +3375,10 @@
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
       <c r="Q5" s="10" t="s">
         <v>20</v>
       </c>
@@ -2072,35 +3412,35 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="59" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="70">
+      <c r="C6" s="54">
         <v>1930</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="54">
         <v>20</v>
       </c>
-      <c r="F6" s="70">
+      <c r="F6" s="54">
         <f>(J6*10^-30)*$K$2*(1*10^6)/4</f>
         <v>26.298218821387195</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70">
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54">
         <v>5.59</v>
       </c>
-      <c r="J6" s="70">
+      <c r="J6" s="54">
         <f>I6^3</f>
         <v>174.67687899999999</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="61" t="s">
         <v>34</v>
       </c>
       <c r="O6" s="23">
@@ -2124,33 +3464,33 @@
       </c>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="62"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="70">
+      <c r="C7" s="54">
         <v>1930</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="70">
+      <c r="E7" s="54">
         <v>78</v>
       </c>
-      <c r="F7" s="70">
+      <c r="F7" s="54">
         <f t="shared" ref="F7:F12" si="0">(J7*10^-30)*$K$2*(1*10^6)/4</f>
         <v>29.07196762444249</v>
       </c>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70">
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54">
         <v>5.78</v>
       </c>
-      <c r="J7" s="70">
+      <c r="J7" s="54">
         <f t="shared" ref="J7:J12" si="1">I7^3</f>
         <v>193.10055200000002</v>
       </c>
-      <c r="N7" s="59"/>
+      <c r="N7" s="56"/>
       <c r="O7" s="24">
         <v>1962</v>
       </c>
@@ -2172,33 +3512,33 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="62"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="70">
+      <c r="C8" s="54">
         <v>1932</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="54">
         <v>82</v>
       </c>
-      <c r="F8" s="70">
+      <c r="F8" s="54">
         <f t="shared" si="0"/>
         <v>27.588997395870205</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70">
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54">
         <v>5.68</v>
       </c>
-      <c r="J8" s="70">
+      <c r="J8" s="54">
         <f t="shared" si="1"/>
         <v>183.25043199999999</v>
       </c>
-      <c r="N8" s="59"/>
+      <c r="N8" s="56"/>
       <c r="O8" s="24">
         <v>1962</v>
       </c>
@@ -2220,33 +3560,33 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="62"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="70">
+      <c r="C9" s="54">
         <v>1932</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="54">
         <v>89</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="54">
         <f t="shared" si="0"/>
         <v>27.734970625161669</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70">
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54">
         <v>5.69</v>
       </c>
-      <c r="J9" s="70">
+      <c r="J9" s="54">
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N9" s="59"/>
+      <c r="N9" s="56"/>
       <c r="O9" s="24">
         <v>1962</v>
       </c>
@@ -2268,33 +3608,33 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="62"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="70">
+      <c r="C10" s="54">
         <v>1932</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="70">
+      <c r="E10" s="54">
         <v>92</v>
       </c>
-      <c r="F10" s="70">
+      <c r="F10" s="54">
         <f t="shared" si="0"/>
         <v>27.734970625161669</v>
       </c>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70">
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54">
         <v>5.69</v>
       </c>
-      <c r="J10" s="70">
+      <c r="J10" s="54">
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N10" s="59"/>
+      <c r="N10" s="56"/>
       <c r="O10" s="24">
         <v>1962</v>
       </c>
@@ -2316,7 +3656,7 @@
       </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="56" t="s">
         <v>38</v>
       </c>
       <c r="C11">
@@ -2339,7 +3679,7 @@
         <f t="shared" si="1"/>
         <v>186.16941100000003</v>
       </c>
-      <c r="N11" s="59"/>
+      <c r="N11" s="56"/>
       <c r="O11" s="24">
         <v>1962</v>
       </c>
@@ -2361,7 +3701,7 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="B12" s="59"/>
+      <c r="B12" s="56"/>
       <c r="C12">
         <v>1957</v>
       </c>
@@ -2382,7 +3722,7 @@
         <f t="shared" si="1"/>
         <v>188.52678690400001</v>
       </c>
-      <c r="N12" s="59"/>
+      <c r="N12" s="56"/>
       <c r="O12" s="24">
         <v>1962</v>
       </c>
@@ -2422,7 +3762,7 @@
       <c r="F13">
         <v>29.65</v>
       </c>
-      <c r="N13" s="59"/>
+      <c r="N13" s="56"/>
       <c r="O13" s="24">
         <v>1962</v>
       </c>
@@ -2444,10 +3784,10 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="56" t="s">
         <v>43</v>
       </c>
       <c r="C14">
@@ -2491,8 +3831,8 @@
       </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
       <c r="C15">
         <v>1960</v>
       </c>
@@ -2531,8 +3871,8 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="58"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
       <c r="C16">
         <v>1960</v>
       </c>
@@ -2571,8 +3911,8 @@
       </c>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="58"/>
-      <c r="B17" s="59"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="56"/>
       <c r="C17">
         <v>1960</v>
       </c>
@@ -2595,8 +3935,8 @@
       <c r="P17" s="24"/>
     </row>
     <row r="18" spans="1:31">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="56"/>
       <c r="C18">
         <v>1960</v>
       </c>
@@ -7365,6 +8705,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="P3:P5"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="Z3:AA3"/>
@@ -7381,11 +8726,6 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="U3:X3"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="P3:P5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N6" r:id="rId1" xr:uid="{19CE446B-6698-4AD9-8C8B-B0EA1227F079}"/>
@@ -7401,6 +8741,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -7424,97 +8765,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="21" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="56" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="64"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="60" t="s">
+      <c r="H5" s="58" t="s">
         <v>81</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" s="11" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A6" s="65"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+      <c r="A6" s="63"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
       <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9">
@@ -8924,104 +10265,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="21" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:18" s="15" customFormat="1">
       <c r="A2" s="14"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="56" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="56"/>
+      <c r="G3" s="57"/>
       <c r="H3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="N3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="56" t="s">
+      <c r="P3" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="56" t="s">
+      <c r="Q3" s="57" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
       <c r="H4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -9037,9 +10378,9 @@
       <c r="I5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -10746,75 +12087,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="21" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:18" s="14" customFormat="1">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
     </row>
     <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="56" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
     </row>
     <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="6" t="s">
         <v>107</v>
       </c>
@@ -10824,17 +12165,17 @@
       <c r="K4" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -10850,9 +12191,9 @@
       <c r="J5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -13418,6 +14759,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:K3"/>
@@ -13426,12 +14773,6 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13463,79 +14804,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1">
       <c r="A2" s="14"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" spans="1:15" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="56" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -13551,8 +14892,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
       <c r="L5" s="10"/>
       <c r="M5" s="13"/>
       <c r="N5" s="16"/>
@@ -22155,85 +23496,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="21" customFormat="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:16" s="15" customFormat="1">
       <c r="A2" s="14"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="56" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="57" t="s">
         <v>155</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
     </row>
     <row r="5" spans="1:16" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -22249,8 +23590,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
       <c r="L5" s="10" t="s">
         <v>28</v>
       </c>
@@ -23904,63 +25245,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="21" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:18" s="15" customFormat="1">
       <c r="A2" s="14"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="56" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
     </row>
     <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
@@ -23976,18 +25317,18 @@
       <c r="I4" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
       <c r="O4" s="6"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24003,9 +25344,9 @@
       <c r="I5" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
       <c r="O5" s="10"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
@@ -24418,6 +25759,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B2:I2"/>
@@ -24425,11 +25771,6 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -24464,39 +25805,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="21" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:18" s="14" customFormat="1">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
     </row>
     <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="56" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -24505,30 +25846,30 @@
       <c r="F3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="N3" s="57" t="s">
         <v>7</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="56" t="s">
+      <c r="P3" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="56" t="s">
+      <c r="Q3" s="57" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
@@ -24537,20 +25878,20 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24566,9 +25907,9 @@
       <c r="I5" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24769,17 +26110,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
krypton high pressure fitted
</commit_message>
<xml_diff>
--- a/data/MASTER Krypton Literature Review.xlsx
+++ b/data/MASTER Krypton Literature Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23059859_student_uwa_edu_au/Documents/UWA/05. Year 5/Semester 1/GENG5511 MPE Engineering Research Project/Project/Research_Project/GENG5511_Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A20B1D7-7FE2-42CA-B3BF-1AB04032541B}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{B44DC191-5C1A-164A-8ECA-80A761F944C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C449EF8-317A-4375-8ABE-0ADCC4BF8EC5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="6" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69D65117-2E76-C546-90A2-B362171284DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell Volume " sheetId="1" r:id="rId1"/>
@@ -1403,23 +1403,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1438,6 +1429,15 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4071,17 +4071,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F513A9-1C82-3E45-A361-2C7180831D5E}">
   <dimension ref="A1:AE136"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AA106" sqref="AA106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="6.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
@@ -4091,14 +4091,14 @@
     <col min="11" max="11" width="12.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.08203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.75" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.25" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.58203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.25" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.5" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="4.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.5" bestFit="1" customWidth="1"/>
@@ -4106,18 +4106,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
       <c r="K1" s="26" t="s">
         <v>1</v>
       </c>
@@ -4142,17 +4142,17 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="5"/>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
       <c r="K2" s="2">
         <f>6.02214076*10^23</f>
         <v>6.0221407599999999E+23</v>
@@ -4177,7 +4177,7 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="63" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="58" t="s">
@@ -4205,7 +4205,7 @@
       <c r="J3" s="58"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="66" t="s">
+      <c r="M3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="58" t="s">
@@ -4239,8 +4239,8 @@
       </c>
       <c r="AA3" s="58"/>
     </row>
-    <row r="4" spans="1:27" ht="16.5">
-      <c r="A4" s="66"/>
+    <row r="4" spans="1:27" ht="18">
+      <c r="A4" s="63"/>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
       <c r="D4" s="58"/>
@@ -4250,10 +4250,10 @@
       <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="62"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="7" t="s">
         <v>17</v>
       </c>
@@ -4262,7 +4262,7 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="66"/>
+      <c r="M4" s="63"/>
       <c r="N4" s="58"/>
       <c r="O4" s="58"/>
       <c r="P4" s="58"/>
@@ -4276,12 +4276,12 @@
         <v>16</v>
       </c>
       <c r="T4" s="7"/>
-      <c r="U4" s="62" t="s">
+      <c r="U4" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="62"/>
-      <c r="W4" s="62"/>
-      <c r="X4" s="62"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
       <c r="Y4" s="27"/>
       <c r="Z4" s="7" t="s">
         <v>17</v>
@@ -4290,11 +4290,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="18.5" thickBot="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+    <row r="5" spans="1:27" ht="18.75" thickBot="1">
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -4315,10 +4315,10 @@
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
       <c r="Q5" s="10" t="s">
         <v>20</v>
       </c>
@@ -4352,7 +4352,7 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="60" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -4380,7 +4380,7 @@
         <f>I6^3</f>
         <v>174.67687899999999</v>
       </c>
-      <c r="N6" s="65" t="s">
+      <c r="N6" s="62" t="s">
         <v>34</v>
       </c>
       <c r="O6" s="23">
@@ -4404,7 +4404,7 @@
       </c>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="64"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="28" t="s">
         <v>32</v>
       </c>
@@ -4430,7 +4430,7 @@
         <f t="shared" ref="J7:J12" si="1">I7^3</f>
         <v>193.10055200000002</v>
       </c>
-      <c r="N7" s="61"/>
+      <c r="N7" s="57"/>
       <c r="O7" s="24">
         <v>1962</v>
       </c>
@@ -4452,7 +4452,7 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="64"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="28" t="s">
         <v>32</v>
       </c>
@@ -4478,7 +4478,7 @@
         <f t="shared" si="1"/>
         <v>183.25043199999999</v>
       </c>
-      <c r="N8" s="61"/>
+      <c r="N8" s="57"/>
       <c r="O8" s="24">
         <v>1962</v>
       </c>
@@ -4500,7 +4500,7 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="64"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
@@ -4526,7 +4526,7 @@
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N9" s="61"/>
+      <c r="N9" s="57"/>
       <c r="O9" s="24">
         <v>1962</v>
       </c>
@@ -4548,7 +4548,7 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="64"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="28" t="s">
         <v>32</v>
       </c>
@@ -4574,7 +4574,7 @@
         <f t="shared" si="1"/>
         <v>184.220009</v>
       </c>
-      <c r="N10" s="61"/>
+      <c r="N10" s="57"/>
       <c r="O10" s="24">
         <v>1962</v>
       </c>
@@ -4596,7 +4596,7 @@
       </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="57" t="s">
         <v>38</v>
       </c>
       <c r="C11">
@@ -4619,7 +4619,7 @@
         <f t="shared" si="1"/>
         <v>186.16941100000003</v>
       </c>
-      <c r="N11" s="61"/>
+      <c r="N11" s="57"/>
       <c r="O11" s="24">
         <v>1962</v>
       </c>
@@ -4641,7 +4641,7 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="B12" s="61"/>
+      <c r="B12" s="57"/>
       <c r="C12">
         <v>1957</v>
       </c>
@@ -4662,7 +4662,7 @@
         <f t="shared" si="1"/>
         <v>188.52678690400001</v>
       </c>
-      <c r="N12" s="61"/>
+      <c r="N12" s="57"/>
       <c r="O12" s="24">
         <v>1962</v>
       </c>
@@ -4702,7 +4702,7 @@
       <c r="F13">
         <v>29.65</v>
       </c>
-      <c r="N13" s="61"/>
+      <c r="N13" s="57"/>
       <c r="O13" s="24">
         <v>1962</v>
       </c>
@@ -4724,10 +4724,10 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="57" t="s">
         <v>43</v>
       </c>
       <c r="C14">
@@ -4771,8 +4771,8 @@
       </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="60"/>
-      <c r="B15" s="61"/>
+      <c r="A15" s="56"/>
+      <c r="B15" s="57"/>
       <c r="C15">
         <v>1960</v>
       </c>
@@ -4811,8 +4811,8 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="60"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16">
         <v>1960</v>
       </c>
@@ -4851,8 +4851,8 @@
       </c>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="60"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="57"/>
       <c r="C17">
         <v>1960</v>
       </c>
@@ -4875,8 +4875,8 @@
       <c r="P17" s="24"/>
     </row>
     <row r="18" spans="1:31">
-      <c r="A18" s="60"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="57"/>
       <c r="C18">
         <v>1960</v>
       </c>
@@ -8705,7 +8705,7 @@
         <v>4.26</v>
       </c>
       <c r="U101">
-        <f t="shared" si="7"/>
+        <f>X101*1000</f>
         <v>4250</v>
       </c>
       <c r="X101">
@@ -9645,6 +9645,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="P3:P5"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="Z3:AA3"/>
@@ -9661,11 +9666,6 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="U3:X3"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="P3:P5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N6" r:id="rId1" xr:uid="{19CE446B-6698-4AD9-8C8B-B0EA1227F079}"/>
@@ -9694,14 +9694,14 @@
       <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="25.58203125" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="13.08203125" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="21" customFormat="1">
@@ -9719,16 +9719,16 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1">
       <c r="A3" s="70" t="s">
@@ -9744,7 +9744,7 @@
       <c r="I3" s="70"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1">
-      <c r="A4" s="66"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="58" t="s">
         <v>5</v>
       </c>
@@ -9764,8 +9764,8 @@
       <c r="H4" s="58"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A5" s="66"/>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="63"/>
       <c r="B5" s="58"/>
       <c r="C5" s="58"/>
       <c r="D5" s="58"/>
@@ -9775,19 +9775,19 @@
       <c r="F5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="G5" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="59" t="s">
         <v>81</v>
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" ht="17" thickBot="1">
-      <c r="A6" s="67"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
+    <row r="6" spans="1:9" s="11" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A6" s="64"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
@@ -11182,25 +11182,25 @@
       <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
     <col min="2" max="2" width="12.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.375" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.75" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.875" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.75" style="18"/>
     <col min="12" max="12" width="12.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.375" style="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.75" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.875" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.08203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.08203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.125" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
@@ -11230,8 +11230,8 @@
       <c r="H2" s="71"/>
       <c r="I2" s="71"/>
     </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="66"/>
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="63"/>
       <c r="B3" s="58" t="s">
         <v>5</v>
       </c>
@@ -11273,8 +11273,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="66"/>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="63"/>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
       <c r="D4" s="58"/>
@@ -11298,11 +11298,11 @@
       <c r="P4" s="58"/>
       <c r="Q4" s="58"/>
     </row>
-    <row r="5" spans="1:18" s="17" customFormat="1" ht="18" thickBot="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+    <row r="5" spans="1:18" s="17" customFormat="1" ht="19.5" thickBot="1">
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -11318,9 +11318,9 @@
       <c r="I5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -13009,20 +13009,20 @@
       <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
@@ -13052,8 +13052,8 @@
       <c r="H2" s="71"/>
       <c r="I2" s="71"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="66"/>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="63"/>
       <c r="B3" s="58" t="s">
         <v>5</v>
       </c>
@@ -13084,8 +13084,8 @@
       <c r="P3" s="58"/>
       <c r="Q3" s="58"/>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="66"/>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="63"/>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
       <c r="D4" s="58"/>
@@ -13113,10 +13113,10 @@
       <c r="Q4" s="58"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -13132,9 +13132,9 @@
       <c r="J5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -15700,6 +15700,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:K3"/>
@@ -15708,12 +15714,6 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -15729,33 +15729,33 @@
       <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.08203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.125" style="18" customWidth="1"/>
     <col min="7" max="11" width="10.75" style="18"/>
     <col min="12" max="12" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.75" style="18"/>
-    <col min="14" max="14" width="12.58203125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="12.625" style="18" customWidth="1"/>
     <col min="15" max="15" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1">
       <c r="A2" s="14"/>
@@ -15767,8 +15767,8 @@
       <c r="E2" s="71"/>
       <c r="F2" s="71"/>
     </row>
-    <row r="3" spans="1:15" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="66"/>
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="63"/>
       <c r="B3" s="58" t="s">
         <v>5</v>
       </c>
@@ -15793,19 +15793,19 @@
       <c r="M3" s="58"/>
       <c r="N3" s="58"/>
     </row>
-    <row r="4" spans="1:15" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="66"/>
+    <row r="4" spans="1:15" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="63"/>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
       <c r="D4" s="58"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="8"/>
       <c r="J4" s="58"/>
       <c r="K4" s="58"/>
@@ -15814,10 +15814,10 @@
       <c r="N4" s="58"/>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -15833,8 +15833,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
       <c r="L5" s="10"/>
       <c r="M5" s="13"/>
       <c r="N5" s="16"/>
@@ -21912,7 +21912,7 @@
         <v>545.16</v>
       </c>
     </row>
-    <row r="345" spans="2:9" customFormat="1" ht="28">
+    <row r="345" spans="2:9" customFormat="1" ht="28.5">
       <c r="B345" s="48" t="s">
         <v>129</v>
       </c>
@@ -22635,7 +22635,7 @@
         <v>143.96</v>
       </c>
     </row>
-    <row r="385" spans="2:7" customFormat="1" ht="29">
+    <row r="385" spans="2:7" customFormat="1" ht="30">
       <c r="B385" s="49" t="s">
         <v>130</v>
       </c>
@@ -24420,34 +24420,34 @@
       <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
     <col min="6" max="6" width="12" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
     <col min="8" max="12" width="10.75" style="18"/>
     <col min="13" max="13" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.75" style="18"/>
-    <col min="15" max="15" width="12.58203125" style="18" customWidth="1"/>
+    <col min="15" max="15" width="12.625" style="18" customWidth="1"/>
     <col min="16" max="16" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.75" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="21" customFormat="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:16" s="15" customFormat="1">
       <c r="A2" s="14"/>
@@ -24459,8 +24459,8 @@
       <c r="E2" s="71"/>
       <c r="F2" s="71"/>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="66"/>
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="63"/>
       <c r="B3" s="58" t="s">
         <v>5</v>
       </c>
@@ -24490,19 +24490,19 @@
       <c r="N3" s="58"/>
       <c r="O3" s="58"/>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="66"/>
+    <row r="4" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="63"/>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
       <c r="D4" s="58"/>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="8"/>
       <c r="J4" s="58"/>
       <c r="K4" s="58"/>
@@ -24512,10 +24512,10 @@
       <c r="O4" s="58"/>
     </row>
     <row r="5" spans="1:16" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -24531,8 +24531,8 @@
       <c r="I5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
       <c r="L5" s="10" t="s">
         <v>28</v>
       </c>
@@ -26162,25 +26162,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5FF47D-C774-6B45-AE66-2A4B51DD47F5}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A26" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6:E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="17.08203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="17.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
@@ -26211,8 +26211,8 @@
       <c r="H2" s="71"/>
       <c r="I2" s="71"/>
     </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="66"/>
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="63"/>
       <c r="B3" s="58" t="s">
         <v>5</v>
       </c>
@@ -26238,8 +26238,8 @@
       <c r="P3" s="58"/>
       <c r="Q3" s="58"/>
     </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="66"/>
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="63"/>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
       <c r="D4" s="58"/>
@@ -26266,10 +26266,10 @@
       <c r="Q4" s="58"/>
     </row>
     <row r="5" spans="1:18" s="17" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -26285,9 +26285,9 @@
       <c r="I5" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
       <c r="O5" s="10"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="16"/>
@@ -26700,6 +26700,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B2:I2"/>
@@ -26707,11 +26712,6 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -26727,20 +26727,20 @@
       <selection pane="bottomLeft" activeCell="E6" sqref="E6:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="18"/>
-    <col min="2" max="2" width="25.58203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="18" customWidth="1"/>
     <col min="3" max="4" width="10.75" style="18"/>
-    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="18" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.08203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="18" customWidth="1"/>
     <col min="10" max="14" width="10.75" style="18"/>
     <col min="15" max="15" width="11.75" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.75" style="18"/>
-    <col min="17" max="17" width="12.58203125" style="18" customWidth="1"/>
+    <col min="17" max="17" width="12.625" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="18" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.75" style="18"/>
   </cols>
@@ -26770,8 +26770,8 @@
       <c r="H2" s="71"/>
       <c r="I2" s="71"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
-      <c r="A3" s="66"/>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A3" s="63"/>
       <c r="B3" s="58" t="s">
         <v>5</v>
       </c>
@@ -26806,8 +26806,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="66"/>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="63"/>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
       <c r="D4" s="58"/>
@@ -26828,11 +26828,11 @@
       <c r="P4" s="58"/>
       <c r="Q4" s="58"/>
     </row>
-    <row r="5" spans="1:18" s="10" customFormat="1" ht="18" thickBot="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+    <row r="5" spans="1:18" s="10" customFormat="1" ht="19.5" thickBot="1">
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
@@ -26848,9 +26848,9 @@
       <c r="I5" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
       <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
@@ -27051,17 +27051,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -27074,7 +27074,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>